<commit_message>
Add even consumer/industry scenario as suggested by HHue
</commit_message>
<xml_diff>
--- a/data/consumer-savings-calculation.xlsx
+++ b/data/consumer-savings-calculation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20386"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20387"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\cpn\app\stop-gas-imports\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\stop-gas-imports\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39FB3595-50F6-4FA1-95F2-6653E6FE0171}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B642752-7F62-4349-B8A2-5533531239C3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="9600" windowHeight="420" xr2:uid="{B2FFA302-30EB-4F26-B634-BB17D3B39911}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="45">
   <si>
     <t>bcm</t>
   </si>
@@ -713,10 +713,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{772CFFD6-E316-4FCB-A61D-92E630F3B5C4}">
-  <dimension ref="A2:K35"/>
+  <dimension ref="A2:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24:K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -924,7 +924,7 @@
         <v>1917.1000000000004</v>
       </c>
       <c r="I20" s="12">
-        <f>eu_industry*F20+H20</f>
+        <f t="shared" ref="I20:I37" si="1">eu_industry*F20+H20</f>
         <v>2643.1000000000004</v>
       </c>
       <c r="J20" s="11">
@@ -964,7 +964,7 @@
         <v>1073.1000000000004</v>
       </c>
       <c r="I21" s="12">
-        <f>eu_industry*F21+H21</f>
+        <f t="shared" si="1"/>
         <v>1799.1000000000004</v>
       </c>
       <c r="J21" s="11">
@@ -1004,7 +1004,7 @@
         <v>2159.1000000000004</v>
       </c>
       <c r="I22" s="12">
-        <f>eu_industry*F22+H22</f>
+        <f t="shared" si="1"/>
         <v>2643.1000000000004</v>
       </c>
       <c r="J22" s="11">
@@ -1044,7 +1044,7 @@
         <v>1373.7000000000007</v>
       </c>
       <c r="I23" s="12">
-        <f>eu_industry*F23+H23</f>
+        <f t="shared" si="1"/>
         <v>1857.7000000000007</v>
       </c>
       <c r="J23" s="11">
@@ -1064,7 +1064,7 @@
         <v>6</v>
       </c>
       <c r="C24" s="11">
-        <v>0.45</v>
+        <v>0.35</v>
       </c>
       <c r="D24" s="11">
         <v>0.8</v>
@@ -1073,27 +1073,27 @@
         <v>0.2</v>
       </c>
       <c r="F24" s="11">
-        <v>0.12</v>
+        <v>0.22600000000000001</v>
       </c>
       <c r="G24" s="12">
         <f>eu_imports*C24+eu_electricity_nochp*D24+eu_electricity_chp*E24+eu_industry*F24</f>
-        <v>5824.7</v>
+        <v>5762.2</v>
       </c>
       <c r="H24" s="12">
         <f>eu_imports - G24</f>
-        <v>1213.3000000000002</v>
+        <v>1275.8000000000002</v>
       </c>
       <c r="I24" s="12">
-        <f>eu_industry*F24+H24</f>
-        <v>1939.3000000000002</v>
+        <f t="shared" ref="I24:I25" si="2">eu_industry*F24+H24</f>
+        <v>2643.1000000000004</v>
       </c>
       <c r="J24" s="11">
         <f>H24/(eu_household+eu_commercial)</f>
-        <v>0.21512411347517735</v>
+        <v>0.22620567375886527</v>
       </c>
       <c r="K24" s="8">
         <f>(eu_imports - (eu_imports*C24+eu_electricity_nochp*D24++eu_electricity_chp*E24+eu_industry*F24))/(eu_household+eu_commercial)</f>
-        <v>0.21512411347517735</v>
+        <v>0.22620567375886527</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -1104,7 +1104,7 @@
         <v>7</v>
       </c>
       <c r="C25" s="11">
-        <v>0.45</v>
+        <v>0.35</v>
       </c>
       <c r="D25" s="11">
         <v>0.8</v>
@@ -1113,107 +1113,107 @@
         <v>0.2</v>
       </c>
       <c r="F25" s="11">
-        <v>0.12</v>
+        <v>0.22600000000000001</v>
       </c>
       <c r="G25" s="12">
         <f>eur_imports*C25+eur_electricity_nochp*D25+eur_electricity_chp*E25+eur_industry*F25</f>
-        <v>6730.3000000000011</v>
+        <v>6817.49</v>
       </c>
       <c r="H25" s="12">
         <f>eur_imports - G25</f>
-        <v>363.69999999999891</v>
+        <v>276.51000000000022</v>
       </c>
       <c r="I25" s="12">
-        <f>eu_industry*F25+H25</f>
-        <v>1089.6999999999989</v>
+        <f t="shared" si="2"/>
+        <v>1643.8100000000002</v>
       </c>
       <c r="J25" s="11">
         <f>H25/(eur_household+eur_commercial)</f>
-        <v>4.7486617051834303E-2</v>
+        <v>3.6102624363493957E-2</v>
       </c>
       <c r="K25" s="8">
         <f>(eur_imports - (eur_imports*C25+eur_electricity_nochp*D25+eur_electricity_chp*E25+eur_industry*F25))/(eur_household+eur_commercial)</f>
-        <v>4.7486617051834303E-2</v>
+        <v>3.6102624363493957E-2</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
         <v>7</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C26" s="11">
-        <v>0.35</v>
+        <v>0.45</v>
       </c>
       <c r="D26" s="11">
         <v>0.8</v>
       </c>
       <c r="E26" s="11">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="F26" s="11">
         <v>0.12</v>
       </c>
       <c r="G26" s="12">
         <f>eu_imports*C26+eu_electricity_nochp*D26+eu_electricity_chp*E26+eu_industry*F26</f>
-        <v>4794.1000000000004</v>
+        <v>5824.7</v>
       </c>
       <c r="H26" s="12">
         <f>eu_imports - G26</f>
-        <v>2243.8999999999996</v>
+        <v>1213.3000000000002</v>
       </c>
       <c r="I26" s="12">
-        <f>eu_industry*F26+H26</f>
-        <v>2969.8999999999996</v>
+        <f t="shared" si="1"/>
+        <v>1939.3000000000002</v>
       </c>
       <c r="J26" s="11">
         <f>H26/(eu_household+eu_commercial)</f>
-        <v>0.39785460992907795</v>
+        <v>0.21512411347517735</v>
       </c>
       <c r="K26" s="8">
         <f>(eu_imports - (eu_imports*C26+eu_electricity_nochp*D26++eu_electricity_chp*E26+eu_industry*F26))/(eu_household+eu_commercial)</f>
-        <v>0.39785460992907795</v>
+        <v>0.21512411347517735</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="9">
         <v>8</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="14" t="s">
         <v>7</v>
       </c>
       <c r="C27" s="11">
-        <v>0.35</v>
+        <v>0.45</v>
       </c>
       <c r="D27" s="11">
         <v>0.8</v>
       </c>
       <c r="E27" s="11">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="F27" s="11">
         <v>0.12</v>
       </c>
       <c r="G27" s="12">
         <f>eur_imports*C27+eur_electricity_nochp*D27+eur_electricity_chp*E27+eur_industry*F27</f>
-        <v>5667.0999999999995</v>
+        <v>6730.3000000000011</v>
       </c>
       <c r="H27" s="12">
         <f>eur_imports - G27</f>
-        <v>1426.9000000000005</v>
+        <v>363.69999999999891</v>
       </c>
       <c r="I27" s="12">
-        <f>eu_industry*F27+H27</f>
-        <v>2152.9000000000005</v>
+        <f t="shared" si="1"/>
+        <v>1089.6999999999989</v>
       </c>
       <c r="J27" s="11">
         <f>H27/(eur_household+eur_commercial)</f>
-        <v>0.18630369499934724</v>
+        <v>4.7486617051834303E-2</v>
       </c>
       <c r="K27" s="8">
         <f>(eur_imports - (eur_imports*C27+eur_electricity_nochp*D27+eur_electricity_chp*E27+eur_industry*F27))/(eur_household+eur_commercial)</f>
-        <v>0.18630369499934724</v>
+        <v>4.7486617051834303E-2</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -1224,36 +1224,36 @@
         <v>6</v>
       </c>
       <c r="C28" s="11">
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="D28" s="11">
         <v>0.8</v>
       </c>
       <c r="E28" s="11">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="F28" s="11">
         <v>0.12</v>
       </c>
       <c r="G28" s="12">
         <f>eu_imports*C28+eu_electricity_nochp*D28+eu_electricity_chp*E28+eu_industry*F28</f>
-        <v>2657.6000000000004</v>
+        <v>4794.1000000000004</v>
       </c>
       <c r="H28" s="12">
         <f>eu_imports - G28</f>
-        <v>4380.3999999999996</v>
+        <v>2243.8999999999996</v>
       </c>
       <c r="I28" s="12">
-        <f>eu_industry*F28+H28</f>
-        <v>5106.3999999999996</v>
+        <f t="shared" si="1"/>
+        <v>2969.8999999999996</v>
       </c>
       <c r="J28" s="11">
         <f>H28/(eu_household+eu_commercial)</f>
-        <v>0.77666666666666662</v>
+        <v>0.39785460992907795</v>
       </c>
       <c r="K28" s="8">
         <f>(eu_imports - (eu_imports*C28+eu_electricity_nochp*D28++eu_electricity_chp*E28+eu_industry*F28))/(eu_household+eu_commercial)</f>
-        <v>0.77666666666666662</v>
+        <v>0.39785460992907795</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -1264,36 +1264,36 @@
         <v>7</v>
       </c>
       <c r="C29" s="11">
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="D29" s="11">
         <v>0.8</v>
       </c>
       <c r="E29" s="11">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="F29" s="11">
         <v>0.12</v>
       </c>
       <c r="G29" s="12">
         <f>eur_imports*C29+eur_electricity_nochp*D29+eur_electricity_chp*E29+eur_industry*F29</f>
-        <v>3538</v>
+        <v>5667.0999999999995</v>
       </c>
       <c r="H29" s="12">
         <f>eur_imports - G29</f>
-        <v>3556</v>
+        <v>1426.9000000000005</v>
       </c>
       <c r="I29" s="12">
-        <f>eu_industry*F29+H29</f>
-        <v>4282</v>
+        <f t="shared" si="1"/>
+        <v>2152.9000000000005</v>
       </c>
       <c r="J29" s="11">
         <f>H29/(eur_household+eur_commercial)</f>
-        <v>0.46429037733385559</v>
+        <v>0.18630369499934724</v>
       </c>
       <c r="K29" s="8">
         <f>(eur_imports - (eur_imports*C29+eur_electricity_nochp*D29+eur_electricity_chp*E29+eur_industry*F29))/(eur_household+eur_commercial)</f>
-        <v>0.46429037733385559</v>
+        <v>0.18630369499934724</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -1307,33 +1307,33 @@
         <v>0</v>
       </c>
       <c r="D30" s="11">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="E30" s="11">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="F30" s="11">
-        <v>0.08</v>
+        <v>0.12</v>
       </c>
       <c r="G30" s="12">
         <f>eu_imports*C30+eu_electricity_nochp*D30+eu_electricity_chp*E30+eu_industry*F30</f>
-        <v>1487</v>
+        <v>2657.6000000000004</v>
       </c>
       <c r="H30" s="12">
         <f>eu_imports - G30</f>
-        <v>5551</v>
+        <v>4380.3999999999996</v>
       </c>
       <c r="I30" s="12">
-        <f>eu_industry*F30+H30</f>
-        <v>6035</v>
+        <f t="shared" si="1"/>
+        <v>5106.3999999999996</v>
       </c>
       <c r="J30" s="11">
         <f>H30/(eu_household+eu_commercial)</f>
-        <v>0.98421985815602842</v>
+        <v>0.77666666666666662</v>
       </c>
       <c r="K30" s="8">
         <f>(eu_imports - (eu_imports*C30+eu_electricity_nochp*D30++eu_electricity_chp*E30+eu_industry*F30))/(eu_household+eu_commercial)</f>
-        <v>0.98421985815602842</v>
+        <v>0.77666666666666662</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -1347,33 +1347,33 @@
         <v>0</v>
       </c>
       <c r="D31" s="11">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="E31" s="11">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="F31" s="11">
-        <v>0.08</v>
+        <v>0.12</v>
       </c>
       <c r="G31" s="12">
         <f>eur_imports*C31+eur_electricity_nochp*D31+eur_electricity_chp*E31+eur_industry*F31</f>
-        <v>2027.7</v>
+        <v>3538</v>
       </c>
       <c r="H31" s="12">
         <f>eur_imports - G31</f>
-        <v>5066.3</v>
+        <v>3556</v>
       </c>
       <c r="I31" s="12">
-        <f>eu_industry*F31+H31</f>
-        <v>5550.3</v>
+        <f t="shared" si="1"/>
+        <v>4282</v>
       </c>
       <c r="J31" s="11">
         <f>H31/(eur_household+eur_commercial)</f>
-        <v>0.66148322235278756</v>
+        <v>0.46429037733385559</v>
       </c>
       <c r="K31" s="8">
         <f>(eur_imports - (eur_imports*C31+eur_electricity_nochp*D31+eur_electricity_chp*E31+eur_industry*F31))/(eur_household+eur_commercial)</f>
-        <v>0.66148322235278756</v>
+        <v>0.46429037733385559</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -1387,33 +1387,33 @@
         <v>0</v>
       </c>
       <c r="D32" s="11">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E32" s="11">
         <v>0</v>
       </c>
       <c r="F32" s="11">
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="G32" s="12">
         <f>eu_imports*C32+eu_electricity_nochp*D32+eu_electricity_chp*E32+eu_industry*F32</f>
-        <v>0</v>
+        <v>1487</v>
       </c>
       <c r="H32" s="12">
         <f>eu_imports - G32</f>
-        <v>7038</v>
+        <v>5551</v>
       </c>
       <c r="I32" s="12">
-        <f>eu_industry*F32+H32</f>
-        <v>7038</v>
+        <f t="shared" si="1"/>
+        <v>6035</v>
       </c>
       <c r="J32" s="11">
         <f>H32/(eu_household+eu_commercial)</f>
-        <v>1.2478723404255319</v>
+        <v>0.98421985815602842</v>
       </c>
       <c r="K32" s="8">
         <f>(eu_imports - (eu_imports*C32+eu_electricity_nochp*D32++eu_electricity_chp*E32+eu_industry*F32))/(eu_household+eu_commercial)</f>
-        <v>1.2478723404255319</v>
+        <v>0.98421985815602842</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -1427,33 +1427,33 @@
         <v>0</v>
       </c>
       <c r="D33" s="11">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E33" s="11">
         <v>0</v>
       </c>
       <c r="F33" s="11">
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="G33" s="12">
         <f>eur_imports*C33+eur_electricity_nochp*D33+eur_electricity_chp*E33+eur_industry*F33</f>
-        <v>0</v>
+        <v>2027.7</v>
       </c>
       <c r="H33" s="12">
         <f>eur_imports - G33</f>
-        <v>7094</v>
+        <v>5066.3</v>
       </c>
       <c r="I33" s="12">
-        <f>eu_industry*F33+H33</f>
-        <v>7094</v>
+        <f t="shared" si="1"/>
+        <v>5550.3</v>
       </c>
       <c r="J33" s="11">
         <f>H33/(eur_household+eur_commercial)</f>
-        <v>0.92623057840449141</v>
+        <v>0.66148322235278756</v>
       </c>
       <c r="K33" s="8">
         <f>(eur_imports - (eur_imports*C33+eur_electricity_nochp*D33+eur_electricity_chp*E33+eur_industry*F33))/(eur_household+eur_commercial)</f>
-        <v>0.92623057840449141</v>
+        <v>0.66148322235278756</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -1464,36 +1464,36 @@
         <v>6</v>
       </c>
       <c r="C34" s="11">
-        <v>0.45</v>
+        <v>0</v>
       </c>
       <c r="D34" s="11">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="E34" s="11">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="F34" s="11">
-        <v>0.12</v>
+        <v>0</v>
       </c>
       <c r="G34" s="12">
         <f>eu_imports*C34+eu_electricity_nochp*D34+eu_electricity_chp*E34+eu_industry*F34</f>
-        <v>5824.7</v>
+        <v>0</v>
       </c>
       <c r="H34" s="12">
         <f>eu_imports - G34</f>
-        <v>1213.3000000000002</v>
+        <v>7038</v>
       </c>
       <c r="I34" s="12">
-        <f>eu_industry*F34+H34</f>
-        <v>1939.3000000000002</v>
+        <f t="shared" si="1"/>
+        <v>7038</v>
       </c>
       <c r="J34" s="11">
         <f>H34/(eu_household+eu_commercial)</f>
-        <v>0.21512411347517735</v>
+        <v>1.2478723404255319</v>
       </c>
       <c r="K34" s="8">
         <f>(eu_imports - (eu_imports*C34+eu_electricity_nochp*D34++eu_electricity_chp*E34+eu_industry*F34))/(eu_household+eu_commercial)</f>
-        <v>0.21512411347517735</v>
+        <v>1.2478723404255319</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -1504,35 +1504,115 @@
         <v>7</v>
       </c>
       <c r="C35" s="11">
-        <v>0.45</v>
+        <v>0</v>
       </c>
       <c r="D35" s="11">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="E35" s="11">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="F35" s="11">
-        <v>0.12</v>
+        <v>0</v>
       </c>
       <c r="G35" s="12">
         <f>eur_imports*C35+eur_electricity_nochp*D35+eur_electricity_chp*E35+eur_industry*F35</f>
-        <v>6553.4000000000005</v>
+        <v>0</v>
       </c>
       <c r="H35" s="12">
         <f>eur_imports - G35</f>
-        <v>540.59999999999945</v>
+        <v>7094</v>
       </c>
       <c r="I35" s="12">
-        <f>eu_industry*F35+H35</f>
-        <v>1266.5999999999995</v>
+        <f t="shared" si="1"/>
+        <v>7094</v>
       </c>
       <c r="J35" s="11">
         <f>H35/(eur_household+eur_commercial)</f>
-        <v>7.058362710536617E-2</v>
+        <v>0.92623057840449141</v>
       </c>
       <c r="K35" s="8">
         <f>(eur_imports - (eur_imports*C35+eur_electricity_nochp*D35+eur_electricity_chp*E35+eur_industry*F35))/(eur_household+eur_commercial)</f>
+        <v>0.92623057840449141</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="14">
+        <v>17</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" s="11">
+        <v>0.45</v>
+      </c>
+      <c r="D36" s="11">
+        <v>0.8</v>
+      </c>
+      <c r="E36" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="F36" s="11">
+        <v>0.12</v>
+      </c>
+      <c r="G36" s="12">
+        <f>eu_imports*C36+eu_electricity_nochp*D36+eu_electricity_chp*E36+eu_industry*F36</f>
+        <v>5824.7</v>
+      </c>
+      <c r="H36" s="12">
+        <f>eu_imports - G36</f>
+        <v>1213.3000000000002</v>
+      </c>
+      <c r="I36" s="12">
+        <f t="shared" si="1"/>
+        <v>1939.3000000000002</v>
+      </c>
+      <c r="J36" s="11">
+        <f>H36/(eu_household+eu_commercial)</f>
+        <v>0.21512411347517735</v>
+      </c>
+      <c r="K36" s="8">
+        <f>(eu_imports - (eu_imports*C36+eu_electricity_nochp*D36++eu_electricity_chp*E36+eu_industry*F36))/(eu_household+eu_commercial)</f>
+        <v>0.21512411347517735</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="14">
+        <v>18</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" s="11">
+        <v>0.45</v>
+      </c>
+      <c r="D37" s="11">
+        <v>0.8</v>
+      </c>
+      <c r="E37" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="F37" s="11">
+        <v>0.12</v>
+      </c>
+      <c r="G37" s="12">
+        <f>eur_imports*C37+eur_electricity_nochp*D37+eur_electricity_chp*E37+eur_industry*F37</f>
+        <v>6553.4000000000005</v>
+      </c>
+      <c r="H37" s="12">
+        <f>eur_imports - G37</f>
+        <v>540.59999999999945</v>
+      </c>
+      <c r="I37" s="12">
+        <f t="shared" si="1"/>
+        <v>1266.5999999999995</v>
+      </c>
+      <c r="J37" s="11">
+        <f>H37/(eur_household+eur_commercial)</f>
+        <v>7.058362710536617E-2</v>
+      </c>
+      <c r="K37" s="8">
+        <f>(eur_imports - (eur_imports*C37+eur_electricity_nochp*D37+eur_electricity_chp*E37+eur_industry*F37))/(eur_household+eur_commercial)</f>
         <v>7.058362710536617E-2</v>
       </c>
     </row>

</xml_diff>